<commit_message>
add try catch error file format
</commit_message>
<xml_diff>
--- a/empty_aud.xlsx
+++ b/empty_aud.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="366">
   <si>
     <t>num_day</t>
   </si>
@@ -79,868 +79,862 @@
     <t>четная</t>
   </si>
   <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 149 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 110 (С-20) ауд. 112(С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 110 (С-20) ауд. 112(С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 149 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 110 (С-20) ауд. 113 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 110 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
   </si>
   <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 131 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 149 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 112(С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 283 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 259 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 262 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 266а (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 283 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 261 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 283 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 266а (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 259 (С-20) ауд. 266а (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 266а (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 263 (С-20) ауд. 266а (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 269 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 244 (С-20) ауд. 261 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 283 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 273 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 269 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 266а (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 254 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 254 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 257 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275 (С-20) ауд. 285 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 331 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 341 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 334 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 347 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 349б (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 453 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 410 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 449 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 453 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 416 (С-20) ауд. 417 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 453 (С-20) ауд. 457 (С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 453 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 447 (С-20) ауд. 453 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 453 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 453 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 415 (С-20) ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 145Б (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 149 (С-20) ауд. 186 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 188.1 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 114 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 110 (С-20) ауд. 113 (С-20) ауд. 130 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 149 (С-20) ауд. 186 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 186 (С-20) ауд. 188.3 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 114 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 145б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 183 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №3 (С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 117 (С-20) ауд. 111 (С-20) ауд. 112 (С-20) ауд. 113 (С-20) ауд. 114 (С-20) ауд. 128 (С-20) ауд. 130 (С-20) ауд. 131 (С-20) ауд. 135 (С-20) ауд. 139 (С-20) ауд. 143 (С-20) ауд. 145Б (С-20) ауд. 147 (С-20) ауд. 149 (С-20) ауд. 186 (С-20) ауд. 188.1 (С-20) ауд. 188.2 (С-20) ауд. 188.3 (С-20) ауд. 191 (С-20) ауд. 2 (С-20) ауд. 3 (С-20) ауд. 6 (С-20) ауд. №20 (С-20) ауд. №20(С-20) ауд. №9 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 259 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 262 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 259 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 263 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 266б (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 244 (С-20) ауд. 261 (С-20) ауд. 265 (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 262 (С-20) ауд. 266б (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 266б (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 258а (С-20) ауд. 265 (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 258а (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 258а (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 283 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 254 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 208 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 257 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20) ауд. 285 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 262 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 269 (С-20) ауд. 273 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 200 (С-20) ауд. 204 (С-20) ауд. 206 (С-20) ауд. 208 (С-20) ауд. 212 (С-20) ауд. 214(С-20) ауд. 215 (С-20) ауд. 215(С-20) ауд. 228 (С-20) ауд. 228(С-20) ауд. 232 (С-20) ауд. 234 (С-20) ауд. 242 (С-20) ауд. 244 (С-20) ауд. 250 (С-20) ауд. 254 (С-20) ауд. 257 (С-20) ауд. 258а (С-20) ауд. 259 (С-20) ауд. 260 (С-20) ауд. 261 (С-20) ауд. 262 (С-20) ауд. 263 (С-20) ауд. 265 (С-20) ауд. 266а (С-20) ауд. 266б (С-20) ауд. 273 (С-20) ауд. 275 (С-20) ауд. 275(С-20) ауд. 279 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 347 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 372 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 331 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 341 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 381 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 347 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 370 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 370 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 322 (С-20) ауд. 325 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 354 (С-20) ауд. 360 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 365 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 354 (С-20) ауд. 365 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326(С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 348 (С-20) ауд. 354 (С-20) ауд. 361 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 381 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 354 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> аб. 329 (С-20) ауд. 318 (С-20) ауд. 322 (С-20) ауд. 324а (С-20) ауд. 325 (С-20) ауд. 326 (С-20) ауд. 326(С-20) ауд. 328 (С-20) ауд. 330 (С-20) ауд. 330(С-20) ауд. 331 (С-20) ауд. 334 (С-20) ауд. 341 (С-20) ауд. 342(С-20) ауд. 343 (С-20) ауд. 344 (С-20) ауд. 346 (С-20) ауд. 347 (С-20) ауд. 348 (С-20) ауд. 350 (С-20) ауд. 353 (С-20) ауд. 354 (С-20) ауд. 356 (С-20) ауд. 359 (С-20) ауд. 360 (С-20) ауд. 361 (С-20) ауд. 367 (С-20) ауд. 367(С-20) ауд. 369 (С-20) ауд. 370 (С-20) ауд. 372 (С-20) ауд. 375 (С-20) ауд. 379 (С-20) ауд. 381 (С-20) ауд. 389 (С-20) ауд. 399б (С-20) ауд. 399б(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457 (С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 415 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453 (С-20) ауд. 453(С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 433 (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445(С-20) ауд. 447 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409(С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457 (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. 409 (С-20) ауд. 409(С-20) ауд. 410 (С-20) ауд. 415 (С-20) ауд. 416 (С-20) ауд. 417 (С-20) ауд. 418 (С-20) ауд. 425 (С-20) ауд. 425(С-20) ауд. 426а (С-20) ауд. 439 (С-20) ауд. 441 (С-20) ауд. 442 (С-20) ауд. 442(С-20) ауд. 445 (С-20) ауд. 445(С-20) ауд. 446 (С-20) ауд. 447 (С-20) ауд. 449 (С-20) ауд. 451 (С-20) ауд. 451(С-20) ауд. 453(С-20) ауд. 455 (С-20) ауд. 455а (С-20) ауд. 457(С-20) ауд. 459 (С-20) ауд. 463 (С-20) ауд. ЗУС-457 (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> комп. 4/5 (С-20) комп. №6 (С-20)</t>
@@ -967,6 +961,9 @@
     <t xml:space="preserve"> комп. 10 (С-20) комп. 13 (С-20) комп. 4/5 (С-20)</t>
   </si>
   <si>
+    <t xml:space="preserve"> комп. 10 (С-20) комп. 13 (С-20) комп. 185 (С-20) комп. 4/5 (С-20) комп. №6 (С-20)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> комп. 13 (С-20) комп. №6 (С-20)</t>
   </si>
   <si>
@@ -979,15 +976,15 @@
     <t xml:space="preserve"> комп. 10 (С-20) комп. №6 (С-20)</t>
   </si>
   <si>
+    <t xml:space="preserve"> комп. 185 (С-20) комп. 4/5 (С-20) комп. №6 (С-20)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> комп. 185 (С-20) комп. 4/5 (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> комп. 10 (С-20) комп. 185 (С-20) комп. 4/5 (С-20) комп. №6 (С-20)</t>
   </si>
   <si>
-    <t xml:space="preserve"> комп. 10 (С-20) комп. 13 (С-20) комп. 185 (С-20) комп. 4/5 (С-20) комп. №6 (С-20)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> комп. 239а (С-20)</t>
   </si>
   <si>
@@ -1006,15 +1003,21 @@
     <t xml:space="preserve"> комп. 281 (С-20)</t>
   </si>
   <si>
-    <t xml:space="preserve"> комп. 246 (С-20) комп. 281 (С-20)</t>
+    <t xml:space="preserve"> комп. 246 (С-20) комп. 251а (С-20) комп. 281 (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> комп. 239а (С-20) комп. 251а (С-20) комп. 281 (С-20)</t>
   </si>
   <si>
+    <t xml:space="preserve"> комп. 239а (С-20) комп. 246 (С-20) комп. 251а (С-20) комп. 281 (С-20)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> комп. 246 (С-20)</t>
   </si>
   <si>
+    <t xml:space="preserve"> комп. 239а (С-20) комп. 281 (С-20)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> комп. 246 (С-20) комп. 251а (С-20)</t>
   </si>
   <si>
@@ -1036,73 +1039,79 @@
     <t xml:space="preserve"> комп. 320 (С-20) комп. 343 (С-20)</t>
   </si>
   <si>
+    <t xml:space="preserve"> комп. 343 (С-20) комп. 383 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 343 (С-20) комп. 344 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 343 (С-20) комп. 344 (С-20) комп. 349 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 320 (С-20) комп. 343 (С-20) комп. 344 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 344 (С-20)</t>
+  </si>
+  <si>
     <t xml:space="preserve"> комп. 383 (С-20)</t>
   </si>
   <si>
-    <t xml:space="preserve"> комп. 344 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 343 (С-20) комп. 344 (С-20) комп. 349 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 320 (С-20) комп. 343 (С-20) комп. 344 (С-20)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> комп. 344 (С-20) комп. 383 (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> комп. 320 (С-20) комп. 344 (С-20)</t>
   </si>
   <si>
-    <t xml:space="preserve"> комп. 343 (С-20) комп. 344 (С-20)</t>
+    <t xml:space="preserve"> комп. 322 (С-20) комп. 343 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 343 (С-20) комп. 344 (С-20) комп. 349 (С-20) комп. 383 (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> комп. 322 (С-20)</t>
   </si>
   <si>
-    <t xml:space="preserve"> комп. 344 (С-20) комп. 349 (С-20) комп. 383 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 344 (С-20) комп. 349 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 322 (С-20) комп. 343 (С-20) комп. 344 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 322 (С-20) комп. 344 (С-20)</t>
+    <t xml:space="preserve"> комп. 429(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 429 (С-20) комп. 429(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 426а (С-20) комп. 429 (С-20) комп. 429(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 426а (С-20) комп. 429(С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 429 (С-20) комп. 429(С-20) комп. 439 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> комп. 429(С-20) комп. 439 (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> комп. 429 (С-20)</t>
   </si>
   <si>
-    <t xml:space="preserve"> комп. 429(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 429 (С-20) комп. 429(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 426а (С-20) комп. 429 (С-20) комп. 429(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 426а (С-20) комп. 429(С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 429 (С-20) комп. 429(С-20) комп. 439 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 429(С-20) комп. 439 (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> комп. 426а (С-20) комп. 429 (С-20) комп. 429(С-20) комп. 439 (С-20)</t>
+    <t xml:space="preserve"> комп. 426а (С-20) комп. 429 (С-20) комп. 439 (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> а (С-20) ауд. (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> а (С-20) ауд. (С-20) физ. ФОК (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> а (С-20) физ. ФОК (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> а (С-20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ауд. (С-20) физ. ФОК (С-20)</t>
   </si>
   <si>
     <t xml:space="preserve"> ауд. (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ауд. (С-20) физ. ФОК (С-20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> физ. ФОК (С-20)</t>
   </si>
 </sst>
 </file>
@@ -1472,10 +1481,10 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44" style="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="41" style="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="59.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="36.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="36.7109375" style="1" customWidth="1"/>
@@ -1548,10 +1557,10 @@
         <v>237</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>352</v>
@@ -1583,10 +1592,10 @@
         <v>238</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>352</v>
@@ -1618,13 +1627,13 @@
         <v>239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>360</v>
@@ -1653,13 +1662,13 @@
         <v>240</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>360</v>
@@ -1688,13 +1697,13 @@
         <v>241</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>360</v>
@@ -1723,10 +1732,13 @@
         <v>242</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>360</v>
@@ -1755,13 +1767,13 @@
         <v>243</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>360</v>
@@ -1790,16 +1802,16 @@
         <v>244</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>360</v>
@@ -1828,13 +1840,13 @@
         <v>245</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>360</v>
@@ -1863,13 +1875,16 @@
         <v>246</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>360</v>
@@ -1898,13 +1913,16 @@
         <v>247</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1930,16 +1948,16 @@
         <v>248</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>360</v>
@@ -1968,16 +1986,19 @@
         <v>249</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -2003,16 +2024,13 @@
         <v>250</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>360</v>
@@ -2041,16 +2059,16 @@
         <v>251</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>360</v>
@@ -2079,16 +2097,16 @@
         <v>252</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>360</v>
@@ -2117,10 +2135,10 @@
         <v>253</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>360</v>
@@ -2149,13 +2167,13 @@
         <v>254</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>360</v>
@@ -2184,10 +2202,10 @@
         <v>255</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>360</v>
@@ -2216,10 +2234,10 @@
         <v>256</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>360</v>
@@ -2248,16 +2266,16 @@
         <v>257</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>360</v>
@@ -2286,16 +2304,13 @@
         <v>258</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>360</v>
@@ -2327,13 +2342,13 @@
         <v>315</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>361</v>
@@ -2365,13 +2380,13 @@
         <v>315</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>361</v>
@@ -2400,13 +2415,13 @@
         <v>261</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>360</v>
@@ -2435,16 +2450,16 @@
         <v>262</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>331</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>360</v>
@@ -2473,10 +2488,10 @@
         <v>263</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>360</v>
@@ -2505,13 +2520,13 @@
         <v>264</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>360</v>
@@ -2540,13 +2555,13 @@
         <v>265</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M30" s="1" t="s">
         <v>360</v>
@@ -2572,19 +2587,16 @@
         <v>194</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>360</v>
@@ -2610,13 +2622,16 @@
         <v>195</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>360</v>
@@ -2642,16 +2657,19 @@
         <v>196</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M33" s="1" t="s">
         <v>360</v>
@@ -2677,19 +2695,19 @@
         <v>197</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>332</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>360</v>
@@ -2715,16 +2733,19 @@
         <v>198</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>332</v>
       </c>
+      <c r="J35" s="1" t="s">
+        <v>339</v>
+      </c>
       <c r="K35" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>360</v>
@@ -2750,19 +2771,19 @@
         <v>199</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>361</v>
@@ -2788,19 +2809,19 @@
         <v>200</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>362</v>
@@ -2826,19 +2847,19 @@
         <v>201</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>360</v>
@@ -2864,19 +2885,22 @@
         <v>202</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2899,19 +2923,19 @@
         <v>203</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>360</v>
@@ -2937,16 +2961,22 @@
         <v>204</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2969,19 +2999,19 @@
         <v>205</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>326</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>360</v>
@@ -3007,16 +3037,19 @@
         <v>206</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -3039,19 +3072,16 @@
         <v>207</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>360</v>
@@ -3077,16 +3107,16 @@
         <v>208</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>360</v>
@@ -3112,19 +3142,19 @@
         <v>209</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>332</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>360</v>
@@ -3150,19 +3180,19 @@
         <v>210</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>360</v>
@@ -3188,22 +3218,22 @@
         <v>211</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -3226,22 +3256,22 @@
         <v>212</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -3264,22 +3294,22 @@
         <v>213</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -3302,19 +3332,19 @@
         <v>214</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -3337,19 +3367,22 @@
         <v>215</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -3372,16 +3405,16 @@
         <v>216</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>360</v>
@@ -3407,16 +3440,19 @@
         <v>217</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -3439,16 +3475,16 @@
         <v>218</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M55" s="1" t="s">
         <v>360</v>
@@ -3474,19 +3510,22 @@
         <v>219</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -3509,19 +3548,19 @@
         <v>220</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M57" s="1" t="s">
         <v>360</v>
@@ -3547,16 +3586,16 @@
         <v>221</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>360</v>
@@ -3582,19 +3621,19 @@
         <v>222</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M59" s="1" t="s">
         <v>360</v>
@@ -3620,19 +3659,19 @@
         <v>223</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="M60" s="1" t="s">
         <v>360</v>
@@ -3658,19 +3697,19 @@
         <v>224</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M61" s="1" t="s">
         <v>360</v>
@@ -3696,16 +3735,13 @@
         <v>225</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="K62" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>361</v>
@@ -3731,13 +3767,13 @@
         <v>226</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M63" s="1" t="s">
         <v>361</v>
@@ -3763,13 +3799,13 @@
         <v>227</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M64" s="1" t="s">
         <v>361</v>
@@ -3795,10 +3831,10 @@
         <v>228</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M65" s="1" t="s">
         <v>361</v>
@@ -3824,13 +3860,13 @@
         <v>229</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M66" s="1" t="s">
         <v>361</v>
@@ -3856,16 +3892,16 @@
         <v>230</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M67" s="1" t="s">
         <v>361</v>
@@ -3891,13 +3927,13 @@
         <v>231</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>322</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>362</v>
@@ -3923,10 +3959,13 @@
         <v>232</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M69" s="1" t="s">
         <v>362</v>
@@ -3952,19 +3991,16 @@
         <v>233</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M70" s="1" t="s">
         <v>362</v>
@@ -3990,10 +4026,10 @@
         <v>234</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>332</v>
@@ -4002,7 +4038,7 @@
         <v>351</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="M71" s="1" t="s">
         <v>362</v>
@@ -4028,19 +4064,19 @@
         <v>235</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>361</v>
@@ -4066,16 +4102,16 @@
         <v>236</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="K73" s="1" t="s">
         <v>359</v>

</xml_diff>